<commit_message>
Ajout des use case et modification de certaines user story
</commit_message>
<xml_diff>
--- a/administratif/analyse_fonctionnelle/Use Case/1-U-C_AjouterItemListeCourses.xlsx
+++ b/administratif/analyse_fonctionnelle/Use Case/1-U-C_AjouterItemListeCourses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1936994\Desktop\ProjetAndroid\dossier fonctionnel\Use Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{7F48DCA1-39A3-4864-8914-26D1B457A1F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5F3B19-E4EB-48DE-98A6-D086FB5715A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{66442B81-2F62-49FF-B014-7C7BE4E0F1D4}"/>
+    <workbookView xWindow="13668" yWindow="1608" windowWidth="17280" windowHeight="8964" xr2:uid="{66442B81-2F62-49FF-B014-7C7BE4E0F1D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -756,166 +756,166 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FAF187-50A3-41BF-81C2-AC788D6D0778}">
   <dimension ref="E3:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:M17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,129 +1251,129 @@
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="10"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="17"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="11"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="20"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30" t="s">
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="32"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="50"/>
     </row>
     <row r="10" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E10" s="33"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="42"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
     </row>
     <row r="11" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E11" s="33"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="39"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="40"/>
     </row>
     <row r="12" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E12" s="33"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="39"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="40"/>
     </row>
     <row r="13" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="11"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="54"/>
     </row>
     <row r="14" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E14" s="9" t="s">
@@ -1382,74 +1382,74 @@
       <c r="F14" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="11"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E17" s="11"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="16"/>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="59"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="11"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="17"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E20" s="7" t="s">
@@ -1458,120 +1458,120 @@
       <c r="F20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="63"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E21" s="24"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="23"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E22" s="25"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="49"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E23" s="25"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="4">
         <v>3</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="49"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E24" s="25"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="4">
         <v>4</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="49"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="25"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="4">
         <v>5</v>
       </c>
-      <c r="G25" s="47" t="s">
+      <c r="G25" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="34"/>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E26" s="25"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="4">
         <v>6</v>
       </c>
-      <c r="G26" s="47" t="s">
+      <c r="G26" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="49"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="34"/>
     </row>
     <row r="27" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="26"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="5">
         <v>7</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="7" t="s">
@@ -1580,96 +1580,96 @@
       <c r="F28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="53" t="s">
+      <c r="G28" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="54"/>
-      <c r="M28" s="55"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="28"/>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E29" s="24"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="23"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="31"/>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E30" s="25"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="49"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="34"/>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E31" s="25"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="49"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E32" s="25"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="34"/>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E33" s="25"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="49"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E34" s="25"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="49"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="34"/>
     </row>
     <row r="35" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E35" s="26"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="17"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
     </row>
     <row r="36" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
@@ -1695,11 +1695,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:M19"/>
-    <mergeCell ref="G20:M20"/>
-    <mergeCell ref="G27:M27"/>
-    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="F7:M8"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:M15"/>
+    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="G32:M32"/>
+    <mergeCell ref="G33:M33"/>
     <mergeCell ref="G28:M28"/>
     <mergeCell ref="G29:M29"/>
     <mergeCell ref="G30:M30"/>
@@ -1708,33 +1711,30 @@
     <mergeCell ref="J12:M12"/>
     <mergeCell ref="G23:M23"/>
     <mergeCell ref="G22:M22"/>
-    <mergeCell ref="E29:E35"/>
-    <mergeCell ref="G34:M34"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="G32:M32"/>
-    <mergeCell ref="G33:M33"/>
     <mergeCell ref="G21:M21"/>
-    <mergeCell ref="E21:E27"/>
-    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:M17"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="E9:E13"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F11:I11"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:M19"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="G27:M27"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="E9:E13"/>
     <mergeCell ref="G26:M26"/>
     <mergeCell ref="G25:M25"/>
     <mergeCell ref="G24:M24"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F5:M6"/>
-    <mergeCell ref="F7:M8"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>